<commit_message>
V2 update format nums
</commit_message>
<xml_diff>
--- a/Redes-Sociales.xlsx
+++ b/Redes-Sociales.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,15 +440,20 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Seguidores</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Me Gusta</t>
         </is>
@@ -457,34 +462,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>https://www.facebook.com/PandoraEspana/</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Pandora</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>18 mill.</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>18 mill.</t>
+          <t>18.000.000</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>18.000.000</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>https://www.facebook.com/tousjewelry</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Tous Jewelry</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2,4 mill.</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2,4 mill.</t>
+          <t>24.000.000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>24.000.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/AristocrazySpain/</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Aristocrazy</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>115.000</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>112.000</t>
         </is>
       </c>
     </row>
@@ -499,7 +536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,20 +547,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Seguidores</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Seguidos</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Publicaciones</t>
         </is>
@@ -532,44 +574,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>https://www.instagram.com/theofficialpandora/</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>theofficialpandora</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>10,5 M</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>105.000.000</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>66</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>4092</t>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4094</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>https://www.instagram.com/tousjewelry/</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>tousjewelry</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1,9 M</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>19.000.000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>35</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>455</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/aristocrazy/</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>aristocrazy</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>240.000</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2975</t>
         </is>
       </c>
     </row>
@@ -584,7 +663,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,20 +674,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Nombre_Canal</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Subscripciones</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Videos</t>
         </is>
@@ -617,20 +701,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/user/TheOfficialPandora</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>TheOfficialPandora</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>@TheOfficialPandora</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>124 k</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>124.000</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>562</t>
         </is>
@@ -639,22 +728,54 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/user/tousjewelry</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>TOUS</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>@TOUSJEWELRYOFFICIAL</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>26.6 k</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>26.600</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>63</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@MrBeast</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MrBeast</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>@MrBeast</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>242.000.000</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>780</t>
         </is>
       </c>
     </row>
@@ -664,91 +785,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Seguidores</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Siguiendo</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Posts</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Pandora Group</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>14,9 mil</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>476</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>692</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>TOUS Jewelry</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>79,5 mil</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>13,4 mil</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -765,79 +801,194 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Seguidores</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Siguiendo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Me Gusta</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Descripcion</t>
+          <t>Posts</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>theofficialpandor</t>
+          <t>https://twitter.com/PANDORA_Corp</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>Pandora Group</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>149.000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>488</t>
+          <t>476</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Aún no hay descripción corta.</t>
+          <t>692</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>https://twitter.com/tousjewelry</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TOUS Jewelry</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>795.000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>134.000</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Seguidores</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Siguiendo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Me Gusta</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@theofficialpandor</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>theofficialpandor</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>488</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Aún no hay descripción corta.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@tousjewelry</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>tousjewelry</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>268.7K</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>268.800</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>28</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1.4M</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>1.400.000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>A space for self-expression, freedom and play. 
 Come to create a world of joy.</t>

</xml_diff>